<commit_message>
Updated the estimates for the project completion based on the prototype results. The cost estimation was also updated accordingly.
</commit_message>
<xml_diff>
--- a/doc/cost_estimation/costestimation.xlsx
+++ b/doc/cost_estimation/costestimation.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Documents\Software Engineering\doc\cost_estimation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9735"/>
   </bookViews>
@@ -45,9 +50,6 @@
     <t>UI Designer for Android</t>
   </si>
   <si>
-    <t>Web Designer for Android</t>
-  </si>
-  <si>
     <t>Database Administrator</t>
   </si>
   <si>
@@ -85,6 +87,9 @@
   </si>
   <si>
     <t>Projected Total Cost</t>
+  </si>
+  <si>
+    <t>Web Designer for Web Application</t>
   </si>
 </sst>
 </file>
@@ -224,22 +229,22 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="60% - Accent2" xfId="3" builtinId="36"/>
@@ -515,7 +520,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -526,7 +531,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,16 +543,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -559,11 +564,11 @@
         <v>69131</v>
       </c>
       <c r="C2" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2">
         <f>B2/52*C2</f>
-        <v>9306.0961538461524</v>
+        <v>11964.98076923077</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -574,11 +579,11 @@
         <v>69131</v>
       </c>
       <c r="C3" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:D7" si="0">B3/52*C3</f>
-        <v>6647.2115384615381</v>
+        <v>9306.0961538461524</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -589,11 +594,11 @@
         <v>69131</v>
       </c>
       <c r="C4" s="3">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
-        <v>7976.6538461538457</v>
+        <v>13294.423076923076</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -613,22 +618,22 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B6" s="2">
         <v>44894</v>
       </c>
       <c r="C6" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
-        <v>1726.6923076923076</v>
+        <v>4316.7307692307695</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2">
         <v>69263</v>
@@ -649,13 +654,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="7">
+        <v>9</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="5">
         <f>SUM(D2:D7)</f>
-        <v>35901.384615384617</v>
+        <v>49126.961538461532</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -671,22 +676,22 @@
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="8" t="s">
+      <c r="A12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>19</v>
+      <c r="D12" s="6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="2">
         <v>750</v>
@@ -701,7 +706,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="2">
         <v>349</v>
@@ -716,7 +721,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="2">
         <v>1129</v>
@@ -731,7 +736,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="2">
         <v>220</v>
@@ -746,7 +751,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="2">
         <v>17500</v>
@@ -767,11 +772,11 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="7">
+        <v>19</v>
+      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="5">
         <f>SUM(D13:D17)</f>
         <v>24047</v>
       </c>
@@ -783,14 +788,14 @@
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="12">
+      <c r="A21" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="11"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="8">
         <f>D9+D17</f>
-        <v>53401.384615384617</v>
+        <v>66626.961538461532</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added a new sheet to the cost estimation excel document that adds up all the lines of code from all the various components of the prototype. This sheet will be used as a reference to generate the estimated source lines of code for the entire project.
</commit_message>
<xml_diff>
--- a/doc/cost_estimation/costestimation.xlsx
+++ b/doc/cost_estimation/costestimation.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Cost Analysis" sheetId="1" r:id="rId1"/>
+    <sheet name="Source Code Estimation" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>Employee Type</t>
   </si>
@@ -90,6 +91,78 @@
   </si>
   <si>
     <t>Web Designer for Web Application</t>
+  </si>
+  <si>
+    <t>Add Bag Servlet</t>
+  </si>
+  <si>
+    <t>Create Collection Log Servlet</t>
+  </si>
+  <si>
+    <t>Get Logs Servlet</t>
+  </si>
+  <si>
+    <t>Verify User Servlet</t>
+  </si>
+  <si>
+    <t>Lines of Code in Prototype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total </t>
+  </si>
+  <si>
+    <t>Lines of Code In Prototype</t>
+  </si>
+  <si>
+    <t>Add Bag Activity</t>
+  </si>
+  <si>
+    <t>Login Activity</t>
+  </si>
+  <si>
+    <t>Main Options Screen</t>
+  </si>
+  <si>
+    <t>Record Collection Info Screen</t>
+  </si>
+  <si>
+    <t>Lines of XML in Layout File</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Web Application</t>
+  </si>
+  <si>
+    <t>Android Application</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database Application </t>
+  </si>
+  <si>
+    <t>Lines of Javascript in Prototype</t>
+  </si>
+  <si>
+    <t>Lines of HTML</t>
+  </si>
+  <si>
+    <t>Login Page</t>
+  </si>
+  <si>
+    <t>Main Menu Page</t>
+  </si>
+  <si>
+    <t>Log Details</t>
+  </si>
+  <si>
+    <t>Outstanding Logs Page</t>
+  </si>
+  <si>
+    <t>Total Lines of UI Code</t>
+  </si>
+  <si>
+    <t>Total Lines of Business Logic Code</t>
   </si>
 </sst>
 </file>
@@ -99,7 +172,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +211,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -223,7 +304,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -245,6 +326,8 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="60% - Accent2" xfId="3" builtinId="36"/>
@@ -530,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,4 +896,228 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.42578125" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="13">
+        <f xml:space="preserve"> SUM(B2:B5)</f>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10">
+        <v>83</v>
+      </c>
+      <c r="C10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11">
+        <v>171</v>
+      </c>
+      <c r="C11">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12">
+        <v>44</v>
+      </c>
+      <c r="C12">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13">
+        <v>235</v>
+      </c>
+      <c r="C13">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="13">
+        <f>SUM(B10:B13)</f>
+        <v>533</v>
+      </c>
+      <c r="C15" s="13">
+        <f>SUM(C10:C13)</f>
+        <v>262</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18">
+        <v>22</v>
+      </c>
+      <c r="C18">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20">
+        <v>41</v>
+      </c>
+      <c r="C20">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21">
+        <v>61</v>
+      </c>
+      <c r="C21">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="13">
+        <f xml:space="preserve"> SUM(B18:B21)</f>
+        <v>124</v>
+      </c>
+      <c r="C23" s="13">
+        <f>SUM(C18:C21)</f>
+        <v>497</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="14">
+        <f>B23+B7+B15</f>
+        <v>988</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="14">
+        <f>C23+C15</f>
+        <v>759</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
I forgot to include the updated cost estimation excel document in the last commit.
</commit_message>
<xml_diff>
--- a/doc/cost_estimation/costestimation.xlsx
+++ b/doc/cost_estimation/costestimation.xlsx
@@ -33,9 +33,6 @@
     <t>Median Annual Salary</t>
   </si>
   <si>
-    <t>Weeks of Work Required</t>
-  </si>
-  <si>
     <t>Total Cost</t>
   </si>
   <si>
@@ -126,9 +123,6 @@
     <t>Record Collection Info Screen</t>
   </si>
   <si>
-    <t>Lines of XML in Layout File</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -141,9 +135,6 @@
     <t xml:space="preserve">Database Application </t>
   </si>
   <si>
-    <t>Lines of Javascript in Prototype</t>
-  </si>
-  <si>
     <t>Lines of HTML</t>
   </si>
   <si>
@@ -163,6 +154,15 @@
   </si>
   <si>
     <t>Total Lines of Business Logic Code</t>
+  </si>
+  <si>
+    <t>Weeks of Work</t>
+  </si>
+  <si>
+    <t>Lines of XML for Layout</t>
+  </si>
+  <si>
+    <t>Lines of Javascript</t>
   </si>
 </sst>
 </file>
@@ -172,7 +172,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,7 +217,27 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -304,14 +324,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -326,8 +343,12 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="60% - Accent2" xfId="3" builtinId="36"/>
@@ -613,279 +634,279 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D21" sqref="A1:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="1" max="1" width="32" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="B2" s="12">
         <v>69131</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="13">
         <v>9</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="12">
         <f>B2/52*C2</f>
         <v>11964.98076923077</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="A3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="12">
         <v>69131</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="13">
         <v>7</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="12">
         <f t="shared" ref="D3:D7" si="0">B3/52*C3</f>
         <v>9306.0961538461524</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="A4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="12">
         <v>69131</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="13">
         <v>10</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="12">
         <f t="shared" si="0"/>
         <v>13294.423076923076</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="A5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="12">
         <v>62137</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="13">
         <v>3</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="12">
         <f t="shared" si="0"/>
         <v>3584.8269230769229</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="2">
+      <c r="A6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="12">
         <v>44894</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="13">
         <v>5</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="12">
         <f t="shared" si="0"/>
         <v>4316.7307692307695</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2">
+      <c r="A7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="12">
         <v>69263</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="13">
         <v>5</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="12">
         <f t="shared" si="0"/>
         <v>6659.9038461538466</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="5">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="3">
         <f>SUM(D2:D7)</f>
         <v>49126.961538461532</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="2">
+      <c r="B13" s="12">
         <v>750</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="13">
         <v>6</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="12">
         <f>C13*B13</f>
         <v>4500</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="2">
+      <c r="A14" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="12">
         <v>349</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="13">
         <v>2</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="12">
         <f t="shared" ref="D14:D17" si="1">C14*B14</f>
         <v>698</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="2">
+      <c r="A15" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="12">
         <v>1129</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="13">
         <v>1</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="12">
         <f t="shared" si="1"/>
         <v>1129</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="2">
+      <c r="A16" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="12">
         <v>220</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="13">
         <v>1</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="12">
         <f t="shared" si="1"/>
         <v>220</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="2">
+      <c r="A17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="12">
         <v>17500</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="13">
         <v>1</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="12">
         <f t="shared" si="1"/>
         <v>17500</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="5">
+      <c r="A19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="3">
         <f>SUM(D13:D17)</f>
         <v>24047</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="8">
+      <c r="A21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="5">
         <f>D9+D17</f>
         <v>66626.961538461532</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -903,218 +924,256 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="C26" sqref="A1:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.42578125" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="14"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="14">
+        <v>66</v>
+      </c>
+      <c r="C2" s="14"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="14">
+        <v>98</v>
+      </c>
+      <c r="C3" s="14"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="14">
+        <v>96</v>
+      </c>
+      <c r="C4" s="14"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="14">
+        <v>71</v>
+      </c>
+      <c r="C5" s="14"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="13">
+      <c r="B7" s="15">
         <f xml:space="preserve"> SUM(B2:B5)</f>
         <v>331</v>
       </c>
+      <c r="C7" s="14"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="B10" s="14">
+        <v>83</v>
+      </c>
+      <c r="C10" s="14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B10">
-        <v>83</v>
-      </c>
-      <c r="C10">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="14">
+        <v>171</v>
+      </c>
+      <c r="C11" s="14">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B11">
-        <v>171</v>
-      </c>
-      <c r="C11">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="B12" s="14">
+        <v>44</v>
+      </c>
+      <c r="C12" s="14">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B12">
-        <v>44</v>
-      </c>
-      <c r="C12">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="B13" s="14">
+        <v>235</v>
+      </c>
+      <c r="C13" s="14">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B13">
-        <v>235</v>
-      </c>
-      <c r="C13">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="13">
+      <c r="B15" s="15">
         <f>SUM(B10:B13)</f>
         <v>533</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="15">
         <f>SUM(C10:C13)</f>
         <v>262</v>
       </c>
     </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+    </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="6" t="s">
+      <c r="A17" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="14">
+        <v>22</v>
+      </c>
+      <c r="C18" s="14">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="B19" s="14">
+        <v>0</v>
+      </c>
+      <c r="C19" s="14">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="14">
+        <v>41</v>
+      </c>
+      <c r="C20" s="14">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18">
-        <v>22</v>
-      </c>
-      <c r="C18">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20">
-        <v>41</v>
-      </c>
-      <c r="C20">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21">
+      <c r="B21" s="14">
         <v>61</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="14">
         <v>105</v>
       </c>
     </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+    </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="13">
+      <c r="A23" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="15">
         <f xml:space="preserve"> SUM(B18:B21)</f>
         <v>124</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C23" s="15">
         <f>SUM(C18:C21)</f>
         <v>497</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="14">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="15">
         <f>B23+B7+B15</f>
         <v>988</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="B26" s="14">
+      <c r="C25" s="14"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="15">
         <f>C23+C15</f>
         <v>759</v>
       </c>
+      <c r="C26" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>